<commit_message>
Add cleaned_data.csv to docs folder
</commit_message>
<xml_diff>
--- a/reports.xlsx
+++ b/reports.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="260">
   <si>
     <t xml:space="preserve">Crossing ID</t>
   </si>
@@ -85,6 +85,75 @@
     <t xml:space="preserve">I block a roadway for over an hour, I go to jail. You block a roadway for over an hour and nothing happens to you. That doesn't seem fair does it?</t>
   </si>
   <si>
+    <t xml:space="preserve">025017A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HOLBROOK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAVAJO BLVD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAVAJO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BNSF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pedestrians were observed climbing on, over, or through the train cars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I can't eat because of the train I'm going to die starvation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">741542E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHOENIX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">48TH STREET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARICOPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16-30 minutes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">026480N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RIVERSIDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3RD ST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backed up traffic onto freeway offramp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">760753C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GLAMIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ben Hulse Hwy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMPERIAL</t>
+  </si>
+  <si>
     <t xml:space="preserve">057548K</t>
   </si>
   <si>
@@ -100,28 +169,91 @@
     <t xml:space="preserve">LOGAN</t>
   </si>
   <si>
-    <t xml:space="preserve">BNSF</t>
+    <t xml:space="preserve">train blockage to our main entrance to hwy. This has every day and sits on track for over 1 hr. blockage time is only limitd to 15 mins. pls help with this concern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272405C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEST PALM BEACH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36TH STREET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PALM BEACH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FEC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">637584H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WAYCROSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SWEAT ST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WARE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disturbing the peace there is a residential neighborhood here </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Respect people trying to sleep not listening to a locomotive popping off running </t>
+  </si>
+  <si>
+    <t xml:space="preserve">732763H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WADLEY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAIN ST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JEFFERSON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-6 hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">traffic congestion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kids going underneath trains</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fewer customers visiting businesses.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">going over train cars.</t>
   </si>
   <si>
     <t xml:space="preserve">6-12 hours</t>
   </si>
   <si>
-    <t xml:space="preserve">unable to get to doctor app</t>
-  </si>
-  <si>
-    <t xml:space="preserve">244861C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FORT COLLINS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">East Mulberry Road</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LARIMER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16-30 minutes</t>
+    <t xml:space="preserve">ems couldn't get around.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First responders were observed being unable to cross the tracks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">police couldn't get around.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kids doing backflips over train cars.</t>
   </si>
   <si>
     <t xml:space="preserve">064031B</t>
@@ -142,49 +274,37 @@
     <t xml:space="preserve">A moving train</t>
   </si>
   <si>
-    <t xml:space="preserve">607220B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FRUITLAND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NORTH ST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MUSCATINE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This happens all the time in our town. The railroad needs to be fined so maybe they will stop doing this</t>
-  </si>
-  <si>
-    <t xml:space="preserve">065622H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALPHA</t>
+    <t xml:space="preserve">876147V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRADFORD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR C55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRANKLIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-15 minutes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No train was present but the lights and/or gates were activated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is a plank sticking up at this crossing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">004741A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOMAX</t>
   </si>
   <si>
     <t xml:space="preserve">IL</t>
   </si>
   <si>
-    <t xml:space="preserve">WEST D ST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HENRY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can’t get home while riding my bike </t>
-  </si>
-  <si>
-    <t xml:space="preserve">065623P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WEST A ST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Backroad is closed and once again blocking both sides </t>
+    <t xml:space="preserve">HENDERSON</t>
   </si>
   <si>
     <t xml:space="preserve">174001M</t>
@@ -199,30 +319,9 @@
     <t xml:space="preserve">COOK</t>
   </si>
   <si>
-    <t xml:space="preserve">UP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-6 hours</t>
-  </si>
-  <si>
     <t xml:space="preserve">This happens at the least three times a week</t>
   </si>
   <si>
-    <t xml:space="preserve">174935X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VILLA PARK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VILLA AVENUE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DU PAGE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Traffic blocking cross streets </t>
-  </si>
-  <si>
     <t xml:space="preserve">283171G</t>
   </si>
   <si>
@@ -232,67 +331,25 @@
     <t xml:space="preserve">150TH ST</t>
   </si>
   <si>
-    <t xml:space="preserve">CSX</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ambulances to Ingalls UChicago Hospital </t>
   </si>
   <si>
-    <t xml:space="preserve">326761B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MELROSE PARK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JOHN F CUNEO CO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IHB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First responders were observed being unable to cross the tracks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">372138C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FRANKLIN PARK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25TH AVENUE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NIRC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">608844V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHICAGO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">W 94TH ST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">846922E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAUGET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MISSISSIPPI AVENU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ST CLAIR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0-15 minutes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deliver trucks delayed; traffic gridlock</t>
+    <t xml:space="preserve">283177X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HALSTED ST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">309452U</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEMONT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIVATE RD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC</t>
   </si>
   <si>
     <t xml:space="preserve">869223U</t>
@@ -307,9 +364,6 @@
     <t xml:space="preserve">BRC</t>
   </si>
   <si>
-    <t xml:space="preserve">Blocked traffic </t>
-  </si>
-  <si>
     <t xml:space="preserve">154238G</t>
   </si>
   <si>
@@ -325,100 +379,82 @@
     <t xml:space="preserve">SHELBY</t>
   </si>
   <si>
-    <t xml:space="preserve">342442Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DECKER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BANDMILL/MAYS RD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KNOX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">445709Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COFFEYVILLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WILLOW STREET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MONTGOMERY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKOL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No train was present but the lights and/or gates were activated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is is a detour on a two lane roadway and is now backed up to the main hwy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">668612U</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAOLA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Waterworks Road</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MIAMI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">813760M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LINWOOD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Main Street</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LEAVENWORTH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">283801Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BURTON</t>
+    <t xml:space="preserve">478029V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FORT WAYNE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LINDENWOOD AVE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALLEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stopped for at least 30 minutes, still stuck and late for work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">937222A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FAIRDALE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OSBORN YARD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">very long train  but stopped for 10  minutes   restarted   stopped for 15 minutes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">233685B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MONROE</t>
   </si>
   <si>
     <t xml:space="preserve">MI</t>
   </si>
   <si>
-    <t xml:space="preserve">BELSAY RD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GENESEE</t>
+    <t xml:space="preserve">MALL ROAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trains blocking RR crossings in Monroe Mi is a reoccurring problem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">283391C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDWARDSBURG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PINE LAKE RD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CASS</t>
   </si>
   <si>
     <t xml:space="preserve">GTW</t>
   </si>
   <si>
-    <t xml:space="preserve">193459P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MANKATO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3rd Ave</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BLUE EARTH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This train is always making me late for work last time they kept me waiting for an hour and thirty minutes. If they're going to block me and make me super late all the time i am owed compensation, frankly it sounds like the train is beginning to move now, but I still want something done to stop them from sitting on this track forever without letting people pass</t>
+    <t xml:space="preserve">511349J</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAY CITY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WILDER ROAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HESR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constant issue with this railroad </t>
   </si>
   <si>
     <t xml:space="preserve">483904B</t>
@@ -436,15 +472,30 @@
     <t xml:space="preserve">CLAY</t>
   </si>
   <si>
+    <t xml:space="preserve">513303C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARYSVILLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The crossing gates were down and blocking the crossing for 60-90 minutes. CSX was notified. </t>
+  </si>
+  <si>
     <t xml:space="preserve">524075X</t>
   </si>
   <si>
     <t xml:space="preserve">SANDUSKY</t>
   </si>
   <si>
-    <t xml:space="preserve">OH</t>
-  </si>
-  <si>
     <t xml:space="preserve">EDGEWATER AVENUE</t>
   </si>
   <si>
@@ -454,6 +505,30 @@
     <t xml:space="preserve">This is a regular occurrence on this location and it’s in a heavily residential area, making it especially unsafe and impacting many.</t>
   </si>
   <si>
+    <t xml:space="preserve">524707D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHARONVILLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HAUCK ROAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HAMILTON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Occurrence during a.m. rush-hour between 7 and 9 AM and it blocks multiple crossings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">524884H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KEMPER ROAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequent occurrence during AM rush hour between 7-9am</t>
+  </si>
+  <si>
     <t xml:space="preserve">012076P</t>
   </si>
   <si>
@@ -499,25 +574,46 @@
     <t xml:space="preserve">GNBC</t>
   </si>
   <si>
-    <t xml:space="preserve">Pedestrians were observed climbing on, over, or through the train cars</t>
-  </si>
-  <si>
     <t xml:space="preserve">Business customers affected</t>
   </si>
   <si>
+    <t xml:space="preserve">759756B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MILWAUKIE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Southeast Harrison Street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLACKAMAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Didn't visit business</t>
+  </si>
+  <si>
+    <t xml:space="preserve">716741S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GREENVILLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WADDELL ROAD</t>
+  </si>
+  <si>
     <t xml:space="preserve">716742Y</t>
   </si>
   <si>
-    <t xml:space="preserve">GREENVILLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SC</t>
-  </si>
-  <si>
     <t xml:space="preserve">PINE KNOLL ROAD</t>
   </si>
   <si>
-    <t xml:space="preserve">350226B</t>
+    <t xml:space="preserve">340968S</t>
   </si>
   <si>
     <t xml:space="preserve">NASHVILLE</t>
@@ -526,48 +622,24 @@
     <t xml:space="preserve">TN</t>
   </si>
   <si>
-    <t xml:space="preserve">SCOTT AVENUE</t>
+    <t xml:space="preserve">TROUSDALE DRIVE</t>
   </si>
   <si>
     <t xml:space="preserve">DAVIDSON</t>
   </si>
   <si>
-    <t xml:space="preserve">014786J</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FARWELL</t>
+    <t xml:space="preserve">Deliveries delayed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">274645R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAGINAW</t>
   </si>
   <si>
     <t xml:space="preserve">TX</t>
   </si>
   <si>
-    <t xml:space="preserve">FM 0292</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PARMER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Semis parked on highway 84 waiting </t>
-  </si>
-  <si>
-    <t xml:space="preserve">024522R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOLANVILLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JACKRABBIT RD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BELL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">274645R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAGINAW</t>
-  </si>
-  <si>
     <t xml:space="preserve">BAILEY BOSWELL RD</t>
   </si>
   <si>
@@ -577,43 +649,40 @@
     <t xml:space="preserve">Traffice congestion. Train slowed to a stop blocking the intersection</t>
   </si>
   <si>
-    <t xml:space="preserve">448436S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FORT WORTH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WILL ROGERS BLVD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FWWR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">597087T</t>
+    <t xml:space="preserve">288127L</t>
   </si>
   <si>
     <t xml:space="preserve">HOUSTON</t>
   </si>
   <si>
-    <t xml:space="preserve">ROSSLYN DR</t>
+    <t xml:space="preserve">Runnels Street</t>
   </si>
   <si>
     <t xml:space="preserve">HARRIS</t>
   </si>
   <si>
-    <t xml:space="preserve">743695P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STAFFORD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KIRKWOOD ROAD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FORT BEND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Near school zone so school arrival probably disrupted, heavy traffic congestion/gridlock</t>
+    <t xml:space="preserve">Gridlock </t>
+  </si>
+  <si>
+    <t xml:space="preserve">288224V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leeland Street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">288228X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">York Street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Traffic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">745046X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOUTH 75TH STREET</t>
   </si>
   <si>
     <t xml:space="preserve">755640L</t>
@@ -622,43 +691,73 @@
     <t xml:space="preserve">Hirsch Road</t>
   </si>
   <si>
+    <t xml:space="preserve">758264S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIVATE</t>
+  </si>
+  <si>
     <t xml:space="preserve">758545B</t>
   </si>
   <si>
     <t xml:space="preserve">SILVER STREET</t>
   </si>
   <si>
-    <t xml:space="preserve">This train has been in front of our house all evening. I have witness multiple pedestrians climbing over it. Absolutely ridiculous. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">764980W</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KIRBY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Walzem Road</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BEXAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Traffic backed up. Train in opposite track came close to the vehicles driving between arms. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">869716G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COKER UNIT 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PTRA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Once again</t>
-  </si>
-  <si>
-    <t xml:space="preserve">467337V</t>
+    <t xml:space="preserve">859516V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMPSON STREET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6:20am to 9:10am during rush hour, horrible congestion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">859517C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YORK STREET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rush hour gridlock, buses stuck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">859518J</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MILBY STREET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">859519R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Private</t>
+  </si>
+  <si>
+    <t xml:space="preserve">859521S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OAKHURST STREET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">859522Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EASTWOOD STREET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">859523F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOCKWOOD STREET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">859524M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DUMBLE STREET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">467352X</t>
   </si>
   <si>
     <t xml:space="preserve">NORFOLK</t>
@@ -667,25 +766,34 @@
     <t xml:space="preserve">VA</t>
   </si>
   <si>
-    <t xml:space="preserve">COLONIAL AVENUE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The train blocked multiple streets. It would stop, go backwards forwards repeatedly.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">467381H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHESAPEAKE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PORTLOCK ROAD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">467668H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CHESAPEAKE BLVD</t>
+    <t xml:space="preserve">CHURCH STREET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Congestion, gridlock, cars turning around</t>
+  </si>
+  <si>
+    <t xml:space="preserve">467692J</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WESTMINISTER AVENUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concrete company production halted with wasted materials </t>
+  </si>
+  <si>
+    <t xml:space="preserve">623548W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RICHMOND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BELLS RD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RICHMOND CITY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Traffic Jam</t>
   </si>
 </sst>
 </file>
@@ -755,7 +863,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:K79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane state="frozen" ySplit="1" topLeftCell="A2"/>
@@ -766,14 +874,14 @@
     <col min="1" max="1" customWidth="1" width="11.714285714285714" bestFit="1"/>
     <col min="2" max="2" customWidth="1" width="17.714285714285715" bestFit="1"/>
     <col min="3" max="3" customWidth="1" width="5.714285714285714" bestFit="1"/>
-    <col min="4" max="4" customWidth="1" width="18.714285714285715" bestFit="1"/>
-    <col min="5" max="5" customWidth="1" width="11.714285714285714" bestFit="1"/>
+    <col min="4" max="4" customWidth="1" width="25.714285714285715" bestFit="1"/>
+    <col min="5" max="5" customWidth="1" width="13.714285714285714" bestFit="1"/>
     <col min="6" max="6" customWidth="1" width="8.714285714285714" bestFit="1"/>
     <col min="7" max="7" customWidth="1" width="57.714285714285715" bestFit="1"/>
     <col min="8" max="8" customWidth="1" width="13.714285714285714" bestFit="1"/>
     <col min="9" max="9" customWidth="1" width="63.714285714285715" bestFit="1"/>
     <col min="10" max="10" customWidth="1" width="135.71428571428572" bestFit="1"/>
-    <col min="11" max="11" customWidth="1" width="363.7142857142857" bestFit="1"/>
+    <col min="11" max="11" customWidth="1" width="163.71428571428572" bestFit="1"/>
   </cols>
   <sheetData>
     <row r="1" x14ac:dyDescent="0.25">
@@ -901,16 +1009,16 @@
         <v>28</v>
       </c>
       <c r="G4" s="3">
-        <v>45502.333333333336</v>
+        <v>45502.910416666666</v>
       </c>
       <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" t="s">
         <v>29</v>
-      </c>
-      <c r="I4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" t="s">
-        <v>18</v>
       </c>
       <c r="K4" t="s">
         <v>30</v>
@@ -933,13 +1041,13 @@
         <v>34</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G5" s="3">
-        <v>45502.416666666664</v>
+        <v>45503.229166666664</v>
       </c>
       <c r="H5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I5" t="s">
         <v>17</v>
@@ -953,37 +1061,37 @@
     </row>
     <row r="6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" t="s">
         <v>38</v>
-      </c>
-      <c r="D6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" t="s">
-        <v>40</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>28</v>
       </c>
       <c r="G6" s="3">
-        <v>45502.6125</v>
+        <v>45503.375</v>
       </c>
       <c r="H6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" t="s">
         <v>41</v>
-      </c>
-      <c r="J6" t="s">
-        <v>18</v>
-      </c>
-      <c r="K6" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7" x14ac:dyDescent="0.25">
@@ -994,7 +1102,7 @@
         <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
         <v>44</v>
@@ -1003,10 +1111,10 @@
         <v>45</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="G7" s="3">
-        <v>45501.67222222222</v>
+        <v>45502.82638888889</v>
       </c>
       <c r="H7" t="s">
         <v>16</v>
@@ -1018,30 +1126,30 @@
         <v>18</v>
       </c>
       <c r="K7" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" t="s">
         <v>48</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
         <v>49</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>50</v>
-      </c>
-      <c r="D8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" t="s">
-        <v>52</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>28</v>
       </c>
       <c r="G8" s="3">
-        <v>45502.461805555555</v>
+        <v>45503.291666666664</v>
       </c>
       <c r="H8" t="s">
         <v>20</v>
@@ -1053,100 +1161,100 @@
         <v>18</v>
       </c>
       <c r="K8" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="G9" s="3">
-        <v>45502.458333333336</v>
+        <v>45503.424305555556</v>
       </c>
       <c r="H9" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="I9" t="s">
         <v>17</v>
       </c>
       <c r="J9" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="K9" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E10" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="G10" s="3">
-        <v>45502.48055555556</v>
+        <v>45502.92152777778</v>
       </c>
       <c r="H10" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="I10" t="s">
         <v>17</v>
       </c>
       <c r="J10" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="K10" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E11" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="G11" s="3">
-        <v>45502.479166666664</v>
+        <v>45502.919444444444</v>
       </c>
       <c r="H11" t="s">
         <v>20</v>
@@ -1158,345 +1266,345 @@
         <v>18</v>
       </c>
       <c r="K11" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="G12" s="3">
-        <v>45502.479166666664</v>
+        <v>45503.260416666664</v>
       </c>
       <c r="H12" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="I12" t="s">
         <v>17</v>
       </c>
       <c r="J12" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="K12" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D13" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="E13" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="G13" s="3">
-        <v>45502.513194444444</v>
+        <v>45503.256944444445</v>
       </c>
       <c r="H13" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="I13" t="s">
         <v>17</v>
       </c>
       <c r="J13" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="K13" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="G14" s="3">
-        <v>45502.36875</v>
+        <v>45503.25</v>
       </c>
       <c r="H14" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="I14" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="J14" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="K14" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" t="s">
         <v>69</v>
       </c>
-      <c r="B15" t="s">
+      <c r="F15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="3">
+        <v>45503.21875</v>
+      </c>
+      <c r="H15" t="s">
         <v>70</v>
       </c>
-      <c r="C15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" t="s">
-        <v>71</v>
-      </c>
-      <c r="E15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G15" s="3">
-        <v>45502.625</v>
-      </c>
-      <c r="H15" t="s">
-        <v>35</v>
-      </c>
       <c r="I15" t="s">
         <v>17</v>
       </c>
       <c r="J15" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="K15" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="3">
+        <v>45503.125</v>
+      </c>
+      <c r="H16" t="s">
         <v>75</v>
       </c>
-      <c r="C16" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="I16" t="s">
+        <v>17</v>
+      </c>
+      <c r="J16" t="s">
+        <v>21</v>
+      </c>
+      <c r="K16" t="s">
         <v>76</v>
-      </c>
-      <c r="E16" t="s">
-        <v>60</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G16" s="3">
-        <v>45502.2375</v>
-      </c>
-      <c r="H16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I16" t="s">
-        <v>41</v>
-      </c>
-      <c r="J16" t="s">
-        <v>78</v>
-      </c>
-      <c r="K16" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="B17" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D17" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="E17" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>82</v>
+        <v>15</v>
       </c>
       <c r="G17" s="3">
-        <v>45502.23888888889</v>
+        <v>45503.125</v>
       </c>
       <c r="H17" t="s">
-        <v>16</v>
+        <v>70</v>
       </c>
       <c r="I17" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="J17" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="K17" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B18" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D18" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="E18" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>82</v>
+        <v>15</v>
       </c>
       <c r="G18" s="3">
-        <v>45501.67847222222</v>
+        <v>45503.041666666664</v>
       </c>
       <c r="H18" t="s">
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="I18" t="s">
         <v>17</v>
       </c>
       <c r="J18" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="K18" t="s">
-        <v>18</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="D19" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E19" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>90</v>
+        <v>28</v>
       </c>
       <c r="G19" s="3">
-        <v>45502.25</v>
+        <v>45502.6125</v>
       </c>
       <c r="H19" t="s">
-        <v>91</v>
+        <v>36</v>
       </c>
       <c r="I19" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="J19" t="s">
         <v>18</v>
       </c>
       <c r="K19" t="s">
-        <v>92</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B20" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="D20" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E20" t="s">
-        <v>60</v>
+        <v>89</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>96</v>
+        <v>35</v>
       </c>
       <c r="G20" s="3">
-        <v>45502.416666666664</v>
+        <v>45503.354166666664</v>
       </c>
       <c r="H20" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="I20" t="s">
-        <v>17</v>
+        <v>91</v>
       </c>
       <c r="J20" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K20" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B21" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C21" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D21" t="s">
-        <v>101</v>
+        <v>68</v>
       </c>
       <c r="E21" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="G21" s="3">
-        <v>45502.64861111111</v>
+        <v>45502.73263888889</v>
       </c>
       <c r="H21" t="s">
         <v>16</v>
@@ -1513,133 +1621,133 @@
     </row>
     <row r="22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B22" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" t="s">
+        <v>99</v>
+      </c>
+      <c r="E22" t="s">
         <v>100</v>
       </c>
-      <c r="D22" t="s">
-        <v>105</v>
-      </c>
-      <c r="E22" t="s">
-        <v>106</v>
-      </c>
       <c r="F22" s="2" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="G22" s="3">
-        <v>45502.208333333336</v>
+        <v>45502.513194444444</v>
       </c>
       <c r="H22" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="I22" t="s">
         <v>17</v>
       </c>
       <c r="J22" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="K22" t="s">
-        <v>18</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B23" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C23" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="D23" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E23" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="G23" s="3">
-        <v>45502.291666666664</v>
+        <v>45502.72361111111</v>
       </c>
       <c r="H23" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="I23" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="J23" t="s">
-        <v>78</v>
+        <v>21</v>
       </c>
       <c r="K23" t="s">
-        <v>114</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="B24" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="C24" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="D24" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="E24" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="G24" s="3">
-        <v>45501.870833333334</v>
+        <v>45502.625</v>
       </c>
       <c r="H24" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="I24" t="s">
         <v>17</v>
       </c>
       <c r="J24" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="K24" t="s">
-        <v>18</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="B25" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="C25" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="D25" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="E25" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G25" s="3">
-        <v>45502.395833333336</v>
+        <v>45502.68819444445</v>
       </c>
       <c r="H25" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="I25" t="s">
         <v>17</v>
@@ -1653,31 +1761,31 @@
     </row>
     <row r="26" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="B26" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C26" t="s">
-        <v>125</v>
+        <v>95</v>
       </c>
       <c r="D26" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="E26" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="G26" s="3">
-        <v>45501.68125</v>
+        <v>45502.78888888889</v>
       </c>
       <c r="H26" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="I26" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="J26" t="s">
         <v>18</v>
@@ -1688,25 +1796,25 @@
     </row>
     <row r="27" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="B27" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="C27" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="D27" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="E27" t="s">
-        <v>133</v>
+        <v>100</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>61</v>
+        <v>115</v>
       </c>
       <c r="G27" s="3">
-        <v>45501.978472222225</v>
+        <v>45502.87569444445</v>
       </c>
       <c r="H27" t="s">
         <v>16</v>
@@ -1718,30 +1826,30 @@
         <v>18</v>
       </c>
       <c r="K27" t="s">
-        <v>134</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="B28" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="C28" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="D28" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="E28" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="G28" s="3">
-        <v>45502.583333333336</v>
+        <v>45502.64861111111</v>
       </c>
       <c r="H28" t="s">
         <v>16</v>
@@ -1758,28 +1866,28 @@
     </row>
     <row r="29" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="B29" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="C29" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
       <c r="D29" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="E29" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G29" s="3">
-        <v>45502.584027777775</v>
+        <v>45503.32430555556</v>
       </c>
       <c r="H29" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="I29" t="s">
         <v>17</v>
@@ -1788,68 +1896,68 @@
         <v>18</v>
       </c>
       <c r="K29" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="B30" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="C30" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="D30" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="E30" t="s">
-        <v>150</v>
+        <v>69</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="G30" s="3">
-        <v>45502.56527777778</v>
+        <v>45502.677083333336</v>
       </c>
       <c r="H30" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="I30" t="s">
         <v>17</v>
       </c>
       <c r="J30" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="K30" t="s">
-        <v>18</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
       <c r="B31" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
       <c r="C31" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="D31" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="E31" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="G31" s="3">
-        <v>45502.66458333333</v>
+        <v>45503.28472222222</v>
       </c>
       <c r="H31" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="I31" t="s">
         <v>17</v>
@@ -1858,103 +1966,103 @@
         <v>18</v>
       </c>
       <c r="K31" t="s">
-        <v>155</v>
+        <v>135</v>
       </c>
     </row>
     <row r="32" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
       <c r="B32" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
       <c r="C32" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="D32" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
       <c r="E32" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="G32" s="3">
-        <v>45502.5</v>
+        <v>45503.464583333334</v>
       </c>
       <c r="H32" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I32" t="s">
         <v>17</v>
       </c>
       <c r="J32" t="s">
-        <v>161</v>
+        <v>18</v>
       </c>
       <c r="K32" t="s">
-        <v>162</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>163</v>
+        <v>141</v>
       </c>
       <c r="B33" t="s">
-        <v>164</v>
+        <v>142</v>
       </c>
       <c r="C33" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="D33" t="s">
-        <v>166</v>
+        <v>143</v>
       </c>
       <c r="E33" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>15</v>
+        <v>145</v>
       </c>
       <c r="G33" s="3">
-        <v>45502.592361111114</v>
+        <v>45502.92083333333</v>
       </c>
       <c r="H33" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="I33" t="s">
         <v>17</v>
       </c>
       <c r="J33" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="K33" t="s">
-        <v>18</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>167</v>
+        <v>141</v>
       </c>
       <c r="B34" t="s">
-        <v>168</v>
+        <v>142</v>
       </c>
       <c r="C34" t="s">
-        <v>169</v>
+        <v>133</v>
       </c>
       <c r="D34" t="s">
-        <v>170</v>
+        <v>143</v>
       </c>
       <c r="E34" t="s">
-        <v>171</v>
+        <v>144</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>72</v>
+        <v>145</v>
       </c>
       <c r="G34" s="3">
-        <v>45502.333333333336</v>
+        <v>45502.90972222222</v>
       </c>
       <c r="H34" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="I34" t="s">
         <v>17</v>
@@ -1968,28 +2076,28 @@
     </row>
     <row r="35" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="B35" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
       <c r="C35" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="D35" t="s">
-        <v>175</v>
+        <v>150</v>
       </c>
       <c r="E35" t="s">
-        <v>176</v>
+        <v>151</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="G35" s="3">
-        <v>45502.381944444445</v>
+        <v>45502.583333333336</v>
       </c>
       <c r="H35" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
       <c r="I35" t="s">
         <v>17</v>
@@ -1998,68 +2106,68 @@
         <v>18</v>
       </c>
       <c r="K35" t="s">
-        <v>177</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>178</v>
+        <v>152</v>
       </c>
       <c r="B36" t="s">
-        <v>179</v>
+        <v>153</v>
       </c>
       <c r="C36" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="D36" t="s">
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="E36" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="G36" s="3">
-        <v>45502.38263888889</v>
+        <v>45502.65625</v>
       </c>
       <c r="H36" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="I36" t="s">
-        <v>17</v>
+        <v>91</v>
       </c>
       <c r="J36" t="s">
         <v>18</v>
       </c>
       <c r="K36" t="s">
-        <v>18</v>
+        <v>157</v>
       </c>
     </row>
     <row r="37" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="B37" t="s">
-        <v>183</v>
+        <v>159</v>
       </c>
       <c r="C37" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="D37" t="s">
-        <v>184</v>
+        <v>160</v>
       </c>
       <c r="E37" t="s">
-        <v>185</v>
+        <v>161</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="G37" s="3">
-        <v>45502.52013888889</v>
+        <v>45502.584027777775</v>
       </c>
       <c r="H37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I37" t="s">
         <v>17</v>
@@ -2068,33 +2176,33 @@
         <v>18</v>
       </c>
       <c r="K37" t="s">
-        <v>186</v>
+        <v>162</v>
       </c>
     </row>
     <row r="38" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>187</v>
+        <v>163</v>
       </c>
       <c r="B38" t="s">
-        <v>188</v>
+        <v>164</v>
       </c>
       <c r="C38" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="D38" t="s">
-        <v>189</v>
+        <v>165</v>
       </c>
       <c r="E38" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>190</v>
+        <v>15</v>
       </c>
       <c r="G38" s="3">
-        <v>45502.34027777778</v>
+        <v>45503.28888888889</v>
       </c>
       <c r="H38" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I38" t="s">
         <v>17</v>
@@ -2103,33 +2211,33 @@
         <v>18</v>
       </c>
       <c r="K38" t="s">
-        <v>18</v>
+        <v>167</v>
       </c>
     </row>
     <row r="39" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
       <c r="B39" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="C39" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="D39" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
       <c r="E39" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="G39" s="3">
-        <v>45501.87291666667</v>
+        <v>45503.28611111111</v>
       </c>
       <c r="H39" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I39" t="s">
         <v>17</v>
@@ -2138,33 +2246,33 @@
         <v>18</v>
       </c>
       <c r="K39" t="s">
-        <v>18</v>
+        <v>170</v>
       </c>
     </row>
     <row r="40" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>195</v>
+        <v>171</v>
       </c>
       <c r="B40" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="C40" t="s">
+        <v>173</v>
+      </c>
+      <c r="D40" t="s">
         <v>174</v>
       </c>
-      <c r="D40" t="s">
-        <v>197</v>
-      </c>
       <c r="E40" t="s">
-        <v>198</v>
+        <v>175</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="G40" s="3">
-        <v>45502.354166666664</v>
+        <v>45502.56527777778</v>
       </c>
       <c r="H40" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="I40" t="s">
         <v>17</v>
@@ -2173,65 +2281,65 @@
         <v>18</v>
       </c>
       <c r="K40" t="s">
-        <v>199</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
       <c r="B41" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="C41" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D41" t="s">
-        <v>201</v>
+        <v>178</v>
       </c>
       <c r="E41" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
       <c r="G41" s="3">
-        <v>45502.350694444445</v>
+        <v>45502.66458333333</v>
       </c>
       <c r="H41" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I41" t="s">
         <v>17</v>
       </c>
       <c r="J41" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K41" t="s">
-        <v>18</v>
+        <v>180</v>
       </c>
     </row>
     <row r="42" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="B42" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="C42" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D42" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="E42" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>61</v>
+        <v>185</v>
       </c>
       <c r="G42" s="3">
-        <v>45502.50347222222</v>
+        <v>45502.5</v>
       </c>
       <c r="H42" t="s">
         <v>20</v>
@@ -2240,77 +2348,77 @@
         <v>17</v>
       </c>
       <c r="J42" t="s">
-        <v>161</v>
+        <v>29</v>
       </c>
       <c r="K42" t="s">
-        <v>18</v>
+        <v>186</v>
       </c>
     </row>
     <row r="43" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="B43" t="s">
+        <v>188</v>
+      </c>
+      <c r="C43" t="s">
+        <v>189</v>
+      </c>
+      <c r="D43" t="s">
+        <v>190</v>
+      </c>
+      <c r="E43" t="s">
+        <v>191</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G43" s="3">
+        <v>45503.42361111111</v>
+      </c>
+      <c r="H43" t="s">
+        <v>36</v>
+      </c>
+      <c r="I43" t="s">
+        <v>17</v>
+      </c>
+      <c r="J43" t="s">
+        <v>18</v>
+      </c>
+      <c r="K43" t="s">
         <v>192</v>
-      </c>
-      <c r="C43" t="s">
-        <v>174</v>
-      </c>
-      <c r="D43" t="s">
-        <v>203</v>
-      </c>
-      <c r="E43" t="s">
-        <v>194</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G43" s="3">
-        <v>45501.88958333333</v>
-      </c>
-      <c r="H43" t="s">
-        <v>29</v>
-      </c>
-      <c r="I43" t="s">
-        <v>17</v>
-      </c>
-      <c r="J43" t="s">
-        <v>161</v>
-      </c>
-      <c r="K43" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="44" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="B44" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C44" t="s">
-        <v>174</v>
+        <v>195</v>
       </c>
       <c r="D44" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="E44" t="s">
         <v>194</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="G44" s="3">
-        <v>45501.876388888886</v>
+        <v>45502.58472222222</v>
       </c>
       <c r="H44" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="I44" t="s">
         <v>17</v>
       </c>
       <c r="J44" t="s">
-        <v>161</v>
+        <v>18</v>
       </c>
       <c r="K44" t="s">
         <v>18</v>
@@ -2318,34 +2426,34 @@
     </row>
     <row r="45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B45" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C45" t="s">
-        <v>174</v>
+        <v>195</v>
       </c>
       <c r="D45" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="E45" t="s">
         <v>194</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="G45" s="3">
-        <v>45501.75069444445</v>
+        <v>45502.592361111114</v>
       </c>
       <c r="H45" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="I45" t="s">
         <v>17</v>
       </c>
       <c r="J45" t="s">
-        <v>161</v>
+        <v>18</v>
       </c>
       <c r="K45" t="s">
         <v>18</v>
@@ -2353,28 +2461,28 @@
     </row>
     <row r="46" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B46" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C46" t="s">
-        <v>174</v>
+        <v>201</v>
       </c>
       <c r="D46" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E46" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G46" s="3">
-        <v>45501.68541666667</v>
+        <v>45503.32986111111</v>
       </c>
       <c r="H46" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="I46" t="s">
         <v>17</v>
@@ -2383,147 +2491,1162 @@
         <v>18</v>
       </c>
       <c r="K46" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="47" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>205</v>
+      </c>
+      <c r="B47" t="s">
+        <v>206</v>
+      </c>
+      <c r="C47" t="s">
+        <v>207</v>
+      </c>
+      <c r="D47" t="s">
+        <v>208</v>
+      </c>
+      <c r="E47" t="s">
+        <v>209</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G47" s="3">
+        <v>45502.52013888889</v>
+      </c>
+      <c r="H47" t="s">
+        <v>90</v>
+      </c>
+      <c r="I47" t="s">
+        <v>17</v>
+      </c>
+      <c r="J47" t="s">
+        <v>18</v>
+      </c>
+      <c r="K47" t="s">
         <v>210</v>
-      </c>
-      <c r="B47" t="s">
-        <v>192</v>
-      </c>
-      <c r="C47" t="s">
-        <v>174</v>
-      </c>
-      <c r="D47" t="s">
-        <v>211</v>
-      </c>
-      <c r="E47" t="s">
-        <v>194</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="G47" s="3">
-        <v>45502.145833333336</v>
-      </c>
-      <c r="H47" t="s">
-        <v>35</v>
-      </c>
-      <c r="I47" t="s">
-        <v>17</v>
-      </c>
-      <c r="J47" t="s">
-        <v>18</v>
-      </c>
-      <c r="K47" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="48" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>211</v>
+      </c>
+      <c r="B48" t="s">
+        <v>212</v>
+      </c>
+      <c r="C48" t="s">
+        <v>207</v>
+      </c>
+      <c r="D48" t="s">
+        <v>213</v>
+      </c>
+      <c r="E48" t="s">
         <v>214</v>
       </c>
-      <c r="B48" t="s">
-        <v>215</v>
-      </c>
-      <c r="C48" t="s">
-        <v>216</v>
-      </c>
-      <c r="D48" t="s">
-        <v>217</v>
-      </c>
-      <c r="E48" t="s">
-        <v>215</v>
-      </c>
       <c r="F48" s="2" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="G48" s="3">
-        <v>45502.354166666664</v>
+        <v>45502.709027777775</v>
       </c>
       <c r="H48" t="s">
         <v>16</v>
       </c>
       <c r="I48" t="s">
-        <v>17</v>
+        <v>91</v>
       </c>
       <c r="J48" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="K48" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="49" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="B49" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="C49" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="D49" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="E49" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="G49" s="3">
-        <v>45501.72222222222</v>
+        <v>45502.70763888889</v>
       </c>
       <c r="H49" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I49" t="s">
-        <v>17</v>
+        <v>91</v>
       </c>
       <c r="J49" t="s">
-        <v>161</v>
+        <v>21</v>
       </c>
       <c r="K49" t="s">
-        <v>18</v>
+        <v>215</v>
       </c>
     </row>
     <row r="50" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>216</v>
+      </c>
+      <c r="B50" t="s">
+        <v>212</v>
+      </c>
+      <c r="C50" t="s">
+        <v>207</v>
+      </c>
+      <c r="D50" t="s">
+        <v>217</v>
+      </c>
+      <c r="E50" t="s">
+        <v>214</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G50" s="3">
+        <v>45502.6875</v>
+      </c>
+      <c r="H50" t="s">
+        <v>70</v>
+      </c>
+      <c r="I50" t="s">
+        <v>17</v>
+      </c>
+      <c r="J50" t="s">
+        <v>29</v>
+      </c>
+      <c r="K50" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>218</v>
+      </c>
+      <c r="B51" t="s">
+        <v>212</v>
+      </c>
+      <c r="C51" t="s">
+        <v>207</v>
+      </c>
+      <c r="D51" t="s">
+        <v>219</v>
+      </c>
+      <c r="E51" t="s">
+        <v>214</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G51" s="3">
+        <v>45502.73263888889</v>
+      </c>
+      <c r="H51" t="s">
+        <v>90</v>
+      </c>
+      <c r="I51" t="s">
+        <v>85</v>
+      </c>
+      <c r="J51" t="s">
+        <v>18</v>
+      </c>
+      <c r="K51" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="52" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>221</v>
+      </c>
+      <c r="B52" t="s">
+        <v>212</v>
+      </c>
+      <c r="C52" t="s">
+        <v>207</v>
+      </c>
+      <c r="D52" t="s">
         <v>222</v>
       </c>
-      <c r="B50" t="s">
+      <c r="E52" t="s">
+        <v>214</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G52" s="3">
+        <v>45502.75347222222</v>
+      </c>
+      <c r="H52" t="s">
+        <v>36</v>
+      </c>
+      <c r="I52" t="s">
+        <v>17</v>
+      </c>
+      <c r="J52" t="s">
+        <v>18</v>
+      </c>
+      <c r="K52" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>223</v>
+      </c>
+      <c r="B53" t="s">
+        <v>212</v>
+      </c>
+      <c r="C53" t="s">
+        <v>207</v>
+      </c>
+      <c r="D53" t="s">
+        <v>224</v>
+      </c>
+      <c r="E53" t="s">
+        <v>214</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G53" s="3">
+        <v>45503.31458333333</v>
+      </c>
+      <c r="H53" t="s">
+        <v>20</v>
+      </c>
+      <c r="I53" t="s">
+        <v>17</v>
+      </c>
+      <c r="J53" t="s">
+        <v>18</v>
+      </c>
+      <c r="K53" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>225</v>
+      </c>
+      <c r="B54" t="s">
+        <v>212</v>
+      </c>
+      <c r="C54" t="s">
+        <v>207</v>
+      </c>
+      <c r="D54" t="s">
+        <v>226</v>
+      </c>
+      <c r="E54" t="s">
+        <v>214</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G54" s="3">
+        <v>45503.333333333336</v>
+      </c>
+      <c r="H54" t="s">
+        <v>70</v>
+      </c>
+      <c r="I54" t="s">
+        <v>17</v>
+      </c>
+      <c r="J54" t="s">
+        <v>18</v>
+      </c>
+      <c r="K54" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>227</v>
+      </c>
+      <c r="B55" t="s">
+        <v>212</v>
+      </c>
+      <c r="C55" t="s">
+        <v>207</v>
+      </c>
+      <c r="D55" t="s">
+        <v>228</v>
+      </c>
+      <c r="E55" t="s">
+        <v>214</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G55" s="3">
+        <v>45502.50347222222</v>
+      </c>
+      <c r="H55" t="s">
+        <v>20</v>
+      </c>
+      <c r="I55" t="s">
+        <v>17</v>
+      </c>
+      <c r="J55" t="s">
+        <v>29</v>
+      </c>
+      <c r="K55" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>229</v>
+      </c>
+      <c r="B56" t="s">
+        <v>212</v>
+      </c>
+      <c r="C56" t="s">
+        <v>207</v>
+      </c>
+      <c r="D56" t="s">
+        <v>230</v>
+      </c>
+      <c r="E56" t="s">
+        <v>214</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G56" s="3">
+        <v>45503.375</v>
+      </c>
+      <c r="H56" t="s">
+        <v>70</v>
+      </c>
+      <c r="I56" t="s">
+        <v>17</v>
+      </c>
+      <c r="J56" t="s">
+        <v>18</v>
+      </c>
+      <c r="K56" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="57" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>229</v>
+      </c>
+      <c r="B57" t="s">
+        <v>212</v>
+      </c>
+      <c r="C57" t="s">
+        <v>207</v>
+      </c>
+      <c r="D57" t="s">
+        <v>230</v>
+      </c>
+      <c r="E57" t="s">
+        <v>214</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G57" s="3">
+        <v>45503.308333333334</v>
+      </c>
+      <c r="H57" t="s">
+        <v>36</v>
+      </c>
+      <c r="I57" t="s">
+        <v>17</v>
+      </c>
+      <c r="J57" t="s">
+        <v>18</v>
+      </c>
+      <c r="K57" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>229</v>
+      </c>
+      <c r="B58" t="s">
+        <v>212</v>
+      </c>
+      <c r="C58" t="s">
+        <v>207</v>
+      </c>
+      <c r="D58" t="s">
+        <v>230</v>
+      </c>
+      <c r="E58" t="s">
+        <v>214</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G58" s="3">
+        <v>45502.73263888889</v>
+      </c>
+      <c r="H58" t="s">
+        <v>16</v>
+      </c>
+      <c r="I58" t="s">
+        <v>17</v>
+      </c>
+      <c r="J58" t="s">
+        <v>21</v>
+      </c>
+      <c r="K58" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="59" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>232</v>
+      </c>
+      <c r="B59" t="s">
+        <v>212</v>
+      </c>
+      <c r="C59" t="s">
+        <v>207</v>
+      </c>
+      <c r="D59" t="s">
+        <v>233</v>
+      </c>
+      <c r="E59" t="s">
+        <v>214</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G59" s="3">
+        <v>45503.375</v>
+      </c>
+      <c r="H59" t="s">
+        <v>70</v>
+      </c>
+      <c r="I59" t="s">
+        <v>17</v>
+      </c>
+      <c r="J59" t="s">
+        <v>18</v>
+      </c>
+      <c r="K59" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="60" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>232</v>
+      </c>
+      <c r="B60" t="s">
+        <v>212</v>
+      </c>
+      <c r="C60" t="s">
+        <v>207</v>
+      </c>
+      <c r="D60" t="s">
+        <v>233</v>
+      </c>
+      <c r="E60" t="s">
+        <v>214</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G60" s="3">
+        <v>45503.30763888889</v>
+      </c>
+      <c r="H60" t="s">
+        <v>36</v>
+      </c>
+      <c r="I60" t="s">
+        <v>17</v>
+      </c>
+      <c r="J60" t="s">
+        <v>18</v>
+      </c>
+      <c r="K60" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>232</v>
+      </c>
+      <c r="B61" t="s">
+        <v>212</v>
+      </c>
+      <c r="C61" t="s">
+        <v>207</v>
+      </c>
+      <c r="D61" t="s">
+        <v>233</v>
+      </c>
+      <c r="E61" t="s">
+        <v>214</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G61" s="3">
+        <v>45503.28194444445</v>
+      </c>
+      <c r="H61" t="s">
+        <v>36</v>
+      </c>
+      <c r="I61" t="s">
+        <v>17</v>
+      </c>
+      <c r="J61" t="s">
+        <v>18</v>
+      </c>
+      <c r="K61" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="62" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>232</v>
+      </c>
+      <c r="B62" t="s">
+        <v>212</v>
+      </c>
+      <c r="C62" t="s">
+        <v>207</v>
+      </c>
+      <c r="D62" t="s">
+        <v>233</v>
+      </c>
+      <c r="E62" t="s">
+        <v>214</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G62" s="3">
+        <v>45503.27847222222</v>
+      </c>
+      <c r="H62" t="s">
+        <v>36</v>
+      </c>
+      <c r="I62" t="s">
+        <v>17</v>
+      </c>
+      <c r="J62" t="s">
+        <v>18</v>
+      </c>
+      <c r="K62" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="63" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>232</v>
+      </c>
+      <c r="B63" t="s">
+        <v>212</v>
+      </c>
+      <c r="C63" t="s">
+        <v>207</v>
+      </c>
+      <c r="D63" t="s">
+        <v>233</v>
+      </c>
+      <c r="E63" t="s">
+        <v>214</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G63" s="3">
+        <v>45502.75069444445</v>
+      </c>
+      <c r="H63" t="s">
+        <v>36</v>
+      </c>
+      <c r="I63" t="s">
+        <v>17</v>
+      </c>
+      <c r="J63" t="s">
+        <v>18</v>
+      </c>
+      <c r="K63" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>232</v>
+      </c>
+      <c r="B64" t="s">
+        <v>212</v>
+      </c>
+      <c r="C64" t="s">
+        <v>207</v>
+      </c>
+      <c r="D64" t="s">
+        <v>233</v>
+      </c>
+      <c r="E64" t="s">
+        <v>214</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G64" s="3">
+        <v>45502.75</v>
+      </c>
+      <c r="H64" t="s">
+        <v>16</v>
+      </c>
+      <c r="I64" t="s">
+        <v>17</v>
+      </c>
+      <c r="J64" t="s">
+        <v>18</v>
+      </c>
+      <c r="K64" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="65" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>232</v>
+      </c>
+      <c r="B65" t="s">
+        <v>212</v>
+      </c>
+      <c r="C65" t="s">
+        <v>207</v>
+      </c>
+      <c r="D65" t="s">
+        <v>233</v>
+      </c>
+      <c r="E65" t="s">
+        <v>214</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G65" s="3">
+        <v>45502.73263888889</v>
+      </c>
+      <c r="H65" t="s">
+        <v>16</v>
+      </c>
+      <c r="I65" t="s">
+        <v>17</v>
+      </c>
+      <c r="J65" t="s">
+        <v>21</v>
+      </c>
+      <c r="K65" t="s">
         <v>215</v>
       </c>
-      <c r="C50" t="s">
-        <v>216</v>
-      </c>
-      <c r="D50" t="s">
-        <v>223</v>
-      </c>
-      <c r="E50" t="s">
-        <v>215</v>
-      </c>
-      <c r="F50" s="2" t="s">
+    </row>
+    <row r="66" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>235</v>
+      </c>
+      <c r="B66" t="s">
+        <v>212</v>
+      </c>
+      <c r="C66" t="s">
+        <v>207</v>
+      </c>
+      <c r="D66" t="s">
+        <v>236</v>
+      </c>
+      <c r="E66" t="s">
+        <v>214</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G66" s="3">
+        <v>45503.375</v>
+      </c>
+      <c r="H66" t="s">
+        <v>70</v>
+      </c>
+      <c r="I66" t="s">
+        <v>17</v>
+      </c>
+      <c r="J66" t="s">
+        <v>18</v>
+      </c>
+      <c r="K66" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="67" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>235</v>
+      </c>
+      <c r="B67" t="s">
+        <v>212</v>
+      </c>
+      <c r="C67" t="s">
+        <v>207</v>
+      </c>
+      <c r="D67" t="s">
+        <v>236</v>
+      </c>
+      <c r="E67" t="s">
+        <v>214</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G67" s="3">
+        <v>45503.27777777778</v>
+      </c>
+      <c r="H67" t="s">
+        <v>36</v>
+      </c>
+      <c r="I67" t="s">
+        <v>17</v>
+      </c>
+      <c r="J67" t="s">
+        <v>18</v>
+      </c>
+      <c r="K67" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>237</v>
+      </c>
+      <c r="B68" t="s">
+        <v>212</v>
+      </c>
+      <c r="C68" t="s">
+        <v>207</v>
+      </c>
+      <c r="D68" t="s">
+        <v>238</v>
+      </c>
+      <c r="E68" t="s">
+        <v>214</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G68" s="3">
+        <v>45503.375</v>
+      </c>
+      <c r="H68" t="s">
+        <v>70</v>
+      </c>
+      <c r="I68" t="s">
+        <v>17</v>
+      </c>
+      <c r="J68" t="s">
+        <v>18</v>
+      </c>
+      <c r="K68" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="69" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>237</v>
+      </c>
+      <c r="B69" t="s">
+        <v>212</v>
+      </c>
+      <c r="C69" t="s">
+        <v>207</v>
+      </c>
+      <c r="D69" t="s">
+        <v>238</v>
+      </c>
+      <c r="E69" t="s">
+        <v>214</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G69" s="3">
+        <v>45503.375</v>
+      </c>
+      <c r="H69" t="s">
+        <v>70</v>
+      </c>
+      <c r="I69" t="s">
+        <v>17</v>
+      </c>
+      <c r="J69" t="s">
+        <v>18</v>
+      </c>
+      <c r="K69" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="70" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>239</v>
+      </c>
+      <c r="B70" t="s">
+        <v>212</v>
+      </c>
+      <c r="C70" t="s">
+        <v>207</v>
+      </c>
+      <c r="D70" t="s">
+        <v>240</v>
+      </c>
+      <c r="E70" t="s">
+        <v>214</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G70" s="3">
+        <v>45503.375</v>
+      </c>
+      <c r="H70" t="s">
+        <v>70</v>
+      </c>
+      <c r="I70" t="s">
+        <v>17</v>
+      </c>
+      <c r="J70" t="s">
+        <v>18</v>
+      </c>
+      <c r="K70" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="71" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>241</v>
+      </c>
+      <c r="B71" t="s">
+        <v>212</v>
+      </c>
+      <c r="C71" t="s">
+        <v>207</v>
+      </c>
+      <c r="D71" t="s">
+        <v>242</v>
+      </c>
+      <c r="E71" t="s">
+        <v>214</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G71" s="3">
+        <v>45503.375</v>
+      </c>
+      <c r="H71" t="s">
+        <v>75</v>
+      </c>
+      <c r="I71" t="s">
+        <v>17</v>
+      </c>
+      <c r="J71" t="s">
+        <v>18</v>
+      </c>
+      <c r="K71" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="72" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>241</v>
+      </c>
+      <c r="B72" t="s">
+        <v>212</v>
+      </c>
+      <c r="C72" t="s">
+        <v>207</v>
+      </c>
+      <c r="D72" t="s">
+        <v>242</v>
+      </c>
+      <c r="E72" t="s">
+        <v>214</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G72" s="3">
+        <v>45503.30694444444</v>
+      </c>
+      <c r="H72" t="s">
+        <v>36</v>
+      </c>
+      <c r="I72" t="s">
+        <v>17</v>
+      </c>
+      <c r="J72" t="s">
+        <v>18</v>
+      </c>
+      <c r="K72" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="73" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>243</v>
+      </c>
+      <c r="B73" t="s">
+        <v>212</v>
+      </c>
+      <c r="C73" t="s">
+        <v>207</v>
+      </c>
+      <c r="D73" t="s">
+        <v>244</v>
+      </c>
+      <c r="E73" t="s">
+        <v>214</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G73" s="3">
+        <v>45503.375</v>
+      </c>
+      <c r="H73" t="s">
+        <v>75</v>
+      </c>
+      <c r="I73" t="s">
+        <v>17</v>
+      </c>
+      <c r="J73" t="s">
+        <v>18</v>
+      </c>
+      <c r="K73" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="74" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>243</v>
+      </c>
+      <c r="B74" t="s">
+        <v>212</v>
+      </c>
+      <c r="C74" t="s">
+        <v>207</v>
+      </c>
+      <c r="D74" t="s">
+        <v>244</v>
+      </c>
+      <c r="E74" t="s">
+        <v>214</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G74" s="3">
+        <v>45502.75</v>
+      </c>
+      <c r="H74" t="s">
+        <v>16</v>
+      </c>
+      <c r="I74" t="s">
+        <v>17</v>
+      </c>
+      <c r="J74" t="s">
+        <v>18</v>
+      </c>
+      <c r="K74" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="75" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>243</v>
+      </c>
+      <c r="B75" t="s">
+        <v>212</v>
+      </c>
+      <c r="C75" t="s">
+        <v>207</v>
+      </c>
+      <c r="D75" t="s">
+        <v>244</v>
+      </c>
+      <c r="E75" t="s">
+        <v>214</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G75" s="3">
+        <v>45502.666666666664</v>
+      </c>
+      <c r="H75" t="s">
+        <v>70</v>
+      </c>
+      <c r="I75" t="s">
+        <v>17</v>
+      </c>
+      <c r="J75" t="s">
+        <v>29</v>
+      </c>
+      <c r="K75" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="76" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>245</v>
+      </c>
+      <c r="B76" t="s">
+        <v>212</v>
+      </c>
+      <c r="C76" t="s">
+        <v>207</v>
+      </c>
+      <c r="D76" t="s">
+        <v>246</v>
+      </c>
+      <c r="E76" t="s">
+        <v>214</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G76" s="3">
+        <v>45503.375</v>
+      </c>
+      <c r="H76" t="s">
+        <v>70</v>
+      </c>
+      <c r="I76" t="s">
+        <v>17</v>
+      </c>
+      <c r="J76" t="s">
+        <v>18</v>
+      </c>
+      <c r="K76" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="77" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>247</v>
+      </c>
+      <c r="B77" t="s">
+        <v>248</v>
+      </c>
+      <c r="C77" t="s">
+        <v>249</v>
+      </c>
+      <c r="D77" t="s">
+        <v>250</v>
+      </c>
+      <c r="E77" t="s">
+        <v>248</v>
+      </c>
+      <c r="F77" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G50" s="3">
-        <v>45502.479166666664</v>
-      </c>
-      <c r="H50" t="s">
-        <v>20</v>
-      </c>
-      <c r="I50" t="s">
-        <v>17</v>
-      </c>
-      <c r="J50" t="s">
-        <v>161</v>
-      </c>
-      <c r="K50" t="s">
-        <v>18</v>
+      <c r="G77" s="3">
+        <v>45503.375</v>
+      </c>
+      <c r="H77" t="s">
+        <v>16</v>
+      </c>
+      <c r="I77" t="s">
+        <v>17</v>
+      </c>
+      <c r="J77" t="s">
+        <v>18</v>
+      </c>
+      <c r="K77" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="78" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>252</v>
+      </c>
+      <c r="B78" t="s">
+        <v>248</v>
+      </c>
+      <c r="C78" t="s">
+        <v>249</v>
+      </c>
+      <c r="D78" t="s">
+        <v>253</v>
+      </c>
+      <c r="E78" t="s">
+        <v>248</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G78" s="3">
+        <v>45503.46527777778</v>
+      </c>
+      <c r="H78" t="s">
+        <v>16</v>
+      </c>
+      <c r="I78" t="s">
+        <v>17</v>
+      </c>
+      <c r="J78" t="s">
+        <v>18</v>
+      </c>
+      <c r="K78" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="79" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>255</v>
+      </c>
+      <c r="B79" t="s">
+        <v>256</v>
+      </c>
+      <c r="C79" t="s">
+        <v>249</v>
+      </c>
+      <c r="D79" t="s">
+        <v>257</v>
+      </c>
+      <c r="E79" t="s">
+        <v>258</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G79" s="3">
+        <v>45502.802083333336</v>
+      </c>
+      <c r="H79" t="s">
+        <v>36</v>
+      </c>
+      <c r="I79" t="s">
+        <v>91</v>
+      </c>
+      <c r="J79" t="s">
+        <v>18</v>
+      </c>
+      <c r="K79" t="s">
+        <v>259</v>
       </c>
     </row>
   </sheetData>

</xml_diff>